<commit_message>
Fix comment with ajax , update file sql
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danhy989\Documents\GitHub\UitTravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5ADD23-4910-4FE1-848F-0625CABDE976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9389AA4-3C2F-4985-8C3A-583CE514F83E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" activeTab="1" xr2:uid="{D398F971-9823-43EE-BF89-8EB1B9B396D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{D398F971-9823-43EE-BF89-8EB1B9B396D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Image</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Detai</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -73,12 +70,6 @@
     <t>Order Image ( Để trống cũng được )</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>Điện Biên</t>
   </si>
   <si>
@@ -275,13 +266,163 @@
   </si>
   <si>
     <t>ID AREA</t>
+  </si>
+  <si>
+    <t>Bãi Biển Mỹ Khê – địa điểm du lịch đẹp ở Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Được mệnh danh là một trong 6 bãi biển đẹp nhất hành tinh nên không thật thiếu sót khi không nhắc đến bãi biển Mỹ Khê. Biển xanh cát vàng mang vẻ đẹp trong trẻo thu hút đông đảo du khách. Chính vì thế khu vực ở đây tập trung rất nhiều nhà hàng khách sạn nhằm phục vụ lượng khách đến Đà Nẵng hàng năm.</t>
+  </si>
+  <si>
+    <t>Bãi Biển Mỹ Khê</t>
+  </si>
+  <si>
+    <t>https://danangaz.com/wp-content/uploads/2018/09/3-min-768x512.jpg</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/bai-bien-my-khe-da-nang2.png</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/bai-bien-my-khe-da-nang3.png</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/bai-tam-my-khe-da-nang1.png</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/nha-hang-syrena-da-nang1.png</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/nha-hang-hai-san-san-ho-da-nang1.png</t>
+  </si>
+  <si>
+    <t>Suối khoáng nóng núi Thần Tài – khu du lịch Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Đây là địa điểm du lịch kết hợp nghỉ dưỡng còn khá mới nhưng nhanh chóng thu hút du khách đến đây. Đến suối khoáng nóng Thần Tài bạn được trải nghiệm không gian nghỉ dưỡng thoải mái với chất lượng dịch vụ đẳng cấp. Tắm suối khoáng ở đây giúp du khách có tinh thần sảng khoái, đầu óc thư giãn.</t>
+  </si>
+  <si>
+    <t> Suối khoáng nóng núi Thần Tài</t>
+  </si>
+  <si>
+    <t>https://danangaz.com/wp-content/uploads/2018/09/4-min-747x420.jpg</t>
+  </si>
+  <si>
+    <t>http://nuithantai.vn/Content/UserFiles/Images/About/th%C3%A1p%20Onsen%201.jpg</t>
+  </si>
+  <si>
+    <t>http://nuithantai.vn/Content/UserFiles/Images/About/C43A2725.JPG</t>
+  </si>
+  <si>
+    <t>Cầu Rồng – địa điểm du lịch Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Cầu Rồng</t>
+  </si>
+  <si>
+    <t>Đà Nẵng nổi tiếng là thành phố của những cây cầu. Bên cạnh biểu tượng lâu đời của thành phố là cầu sông Hàn thì cầu Rồng cũng nổi tiếng chẳng kém. Con rồng khổng lồ màu vàng rực chuyển màu liên tục khi đêm đến vắt ngang qua dòng sông Hàn thơ mộng gây ấn tượng trong lòng du khách.</t>
+  </si>
+  <si>
+    <t>https://danangaz.com/wp-content/uploads/2018/09/5-min-768x383.jpg</t>
+  </si>
+  <si>
+    <t>https://www.tuannguyentravel.com/data/images/cau-rong%281%29.jpg</t>
+  </si>
+  <si>
+    <t>http://www.geoholidayclub.org/wp-content/uploads/2018/02/Hu%E1%BA%BF-%C4%91i-%C4%90%C3%A0-N%E1%BA%B5ng-bao-nhi%C3%AAu-km.jpg</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/c-r-e1505464506291.jpg</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/Cau-rong-da-nang-buoi-chieu-ta.png</t>
+  </si>
+  <si>
+    <t>https://vntrip.cdn.vccloud.vn/cam-nang/wp-content/uploads/2017/07/toan-canh-cau-rong-vo-cung-hoanh-trang.png</t>
+  </si>
+  <si>
+    <t>Cầu Tình Yêu</t>
+  </si>
+  <si>
+    <t>Cầu Tình Yêu – địa điểm đi chơi Đà Nẵng</t>
+  </si>
+  <si>
+    <t>Lại là địa điểm đẹp rất thu hút các cặp đôi đến đây để check in hay móc khóa tình yêu vào cây cầu như minh chứng cho 1 tình yêu đẹp đẽ. Hình ảnh trái tim nối đuôi nhau từ đầu cầu đến cuối cầu rất đẹp.</t>
+  </si>
+  <si>
+    <t>https://danangaz.com/wp-content/uploads/2018/09/6-min.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dulichdanang.biz.vn/_/rsrc/1486448631044/diem-du-lich/cau-tinh-yeu-da-nang/cau-tinh-yeu-da-nang.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dulichdanang.biz.vn/_/rsrc/1486448714514/diem-du-lich/cau-tinh-yeu-da-nang/cau-tinh-yeu-danang.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dulichdanang.biz.vn/_/rsrc/1486449087327/diem-du-lich/cau-tinh-yeu-da-nang/cautinhyeudanang.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dulichdanang.biz.vn/_/rsrc/1486449963961/diem-du-lich/cau-tinh-yeu-da-nang/cau-tinh-yeu-da-nang2.jpg</t>
+  </si>
+  <si>
+    <t>http://www.dulichdanang.biz.vn/_/rsrc/1486450139513/diem-du-lich/cau-tinh-yeu-da-nang/cau-tinh-yeu-da-nang3.jpg</t>
+  </si>
+  <si>
+    <t>Cù Lao Chàm</t>
+  </si>
+  <si>
+    <t>Cù Lao Chàm – địa điểm du lịch khi đến Đà Nẵng</t>
+  </si>
+  <si>
+    <r>
+      <t>Du lịch Cù Lao Chàm là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>địa điểm du lịch Đà Nẵng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> hấp dẫn du khách. Nơi đây được ví là hòn ngọc giữa biển, mang nét đẹp đặc trưng. Đến Cù Lao Chàm, bạn có thể đi đến các địa điểm như chùa Hải Tạng, nhà bảo tàng, giếng cổ Chăm, chợ Tân Hiệp, miếu tổ nghề Yến. Ngoài ra bạn còn được thưởng thức các đặc sản nơi đây như mực một nắng, cua đá, ốc vú nàng… Hứa hẹn chuyến đi có nhiều trải nghiệm thú vị.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://danangaz.com/wp-content/uploads/2018/09/7-min.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn3.ivivu.com/2016/02/dao-cu-lao-cham-ivivu-1.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn3.ivivu.com/2016/02/dao-cu-lao-cham-ivivu-2-1024x571.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn3.ivivu.com/2016/02/dao-cu-lao-cham-ivivu-5.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn3.ivivu.com/2016/02/dao-cu-lao-cham-ivivu-4.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn3.ivivu.com/2016/02/dao-cu-lao-cham-ivivu-6.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +445,48 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -341,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,13 +532,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -674,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA48DFE-8E50-45DB-8934-5324C6EBDBEC}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,188 +883,230 @@
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="12">
+        <v>5500000</v>
+      </c>
+      <c r="F3" s="12">
+        <v>34</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="E4" s="4">
-        <v>1</v>
+        <v>3000000</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>92</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>96</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="E5" s="4">
-        <v>1</v>
+        <v>350000</v>
       </c>
       <c r="F5" s="4">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="2">
+        <v>6000000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2500000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1486,8 +1725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892EC322-56F2-4580-AC70-F0D96901DCF7}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,706 +1737,706 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>79</v>
+      <c r="A1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="C34" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="B47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="C35" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="B48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="C36" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>36</v>
-      </c>
-      <c r="B37" s="6" t="s">
+      <c r="B49" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="C37" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>37</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="B50" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="C38" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
-        <v>38</v>
-      </c>
-      <c r="B39" s="6" t="s">
+      <c r="B51" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
         <v>51</v>
       </c>
-      <c r="C39" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
-        <v>39</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="B52" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
         <v>52</v>
       </c>
-      <c r="C40" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
-        <v>40</v>
-      </c>
-      <c r="B41" s="6" t="s">
+      <c r="B53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
         <v>53</v>
       </c>
-      <c r="C41" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
-        <v>41</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="B54" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
         <v>54</v>
       </c>
-      <c r="C42" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>42</v>
-      </c>
-      <c r="B43" s="6" t="s">
+      <c r="B55" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
         <v>55</v>
       </c>
-      <c r="C43" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="6">
-        <v>43</v>
-      </c>
-      <c r="B44" s="6" t="s">
+      <c r="B56" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
         <v>56</v>
       </c>
-      <c r="C44" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
-        <v>44</v>
-      </c>
-      <c r="B45" s="6" t="s">
+      <c r="B57" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
         <v>57</v>
       </c>
-      <c r="C45" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
-        <v>45</v>
-      </c>
-      <c r="B46" s="6" t="s">
+      <c r="B58" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
         <v>58</v>
       </c>
-      <c r="C46" s="6">
+      <c r="B59" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>46</v>
-      </c>
-      <c r="B47" s="6" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
         <v>59</v>
       </c>
-      <c r="C47" s="6">
+      <c r="B60" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
-        <v>47</v>
-      </c>
-      <c r="B48" s="6" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
         <v>60</v>
       </c>
-      <c r="C48" s="6">
+      <c r="B61" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
         <v>61</v>
       </c>
-      <c r="C49" s="6">
+      <c r="B62" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6">
-        <v>49</v>
-      </c>
-      <c r="B50" s="6" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
         <v>62</v>
       </c>
-      <c r="C50" s="6">
+      <c r="B63" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
-        <v>50</v>
-      </c>
-      <c r="B51" s="6" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
         <v>63</v>
       </c>
-      <c r="C51" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6">
-        <v>51</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
-        <v>52</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6">
-        <v>53</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
-        <v>54</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6">
-        <v>55</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6">
-        <v>56</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C57" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6">
-        <v>57</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6">
-        <v>58</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6">
-        <v>59</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6">
-        <v>60</v>
-      </c>
-      <c r="B61" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6">
-        <v>61</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6">
-        <v>62</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6">
-        <v>63</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="6">
+      <c r="C64" s="5">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
import thêm một số tour
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danhy989\Documents\GitHub\UitTravel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danhy989\Documents\GitHub\uittravel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EAA00B-1F7C-416A-9096-81E9E285566C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F31E866-5123-4D31-B30D-65FF72D944D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{D398F971-9823-43EE-BF89-8EB1B9B396D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,10 @@
     <definedName name="A">Trang_tính1!$A:$A</definedName>
     <definedName name="id">Trang_tính1!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -275,7 +270,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +329,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -367,10 +370,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,12 +389,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -401,9 +399,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -714,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA48DFE-8E50-45DB-8934-5324C6EBDBEC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,39 +752,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
@@ -786,160 +802,160 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="11"/>
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -1464,11 +1480,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892EC322-56F2-4580-AC70-F0D96901DCF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>